<commit_message>
add chernobyl data parser
</commit_message>
<xml_diff>
--- a/wdc_libs/parsers/wdc-timeline/timeline5.6.xlsx
+++ b/wdc_libs/parsers/wdc-timeline/timeline5.6.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="190">
   <si>
     <t>key</t>
   </si>
@@ -592,6 +592,9 @@
   </si>
   <si>
     <t>http://ipress.ua/media/gallery/full/b/o/boeing_777_malaysia_airlines.jpg</t>
+  </si>
+  <si>
+    <t>bla  bla bla</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1136,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.28515625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1192,6 +1195,9 @@
       <c r="C3" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1478,7 +1484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1928,7 +1934,7 @@
   <dimension ref="A1:E846"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>